<commit_message>
5V External Buck Done
</commit_message>
<xml_diff>
--- a/Power_Board_2/Calculations/5V_buck.xlsx
+++ b/Power_Board_2/Calculations/5V_buck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvicca0-my.sharepoint.com/personal/poornack_uvicca0_onmicrosoft_com/Documents/University/Clubs/AUVic/Hardware/PCB-Power_Board_2/Power_Board_2/Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{96FACF96-6EB4-48BA-A4BA-9FAB68A7D684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06C6A0B3-DA3C-49F1-9C0B-AF32DDE05920}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{96FACF96-6EB4-48BA-A4BA-9FAB68A7D684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7CF08298-9F28-453C-91B0-3518F2637AE9}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="16440" xr2:uid="{C6339F42-7D1E-4B11-8B04-09094EF93EB8}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="f_S">Sheet1!$B$7</definedName>
     <definedName name="K">Sheet1!$B$6</definedName>
     <definedName name="R_ON">Sheet1!$B$17</definedName>
+    <definedName name="R_ON_ACT">Sheet1!$B$18</definedName>
     <definedName name="R_OND">Sheet1!$B$16</definedName>
     <definedName name="V_IN">Sheet1!$B$5</definedName>
     <definedName name="V_INMAX">Sheet1!$B$4</definedName>
@@ -35,7 +36,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Calculating R_ON</t>
   </si>
@@ -79,6 +82,12 @@
   </si>
   <si>
     <t>f_SMAX</t>
+  </si>
+  <si>
+    <t>R_ON_ACT</t>
+  </si>
+  <si>
+    <t>t_ON</t>
   </si>
 </sst>
 </file>
@@ -116,10 +125,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10EE0DC-C48A-41CB-95F2-10E1DAB19583}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,11 +455,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -488,7 +497,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1E-10</v>
       </c>
     </row>
@@ -496,7 +505,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>825000</v>
       </c>
     </row>
@@ -543,6 +552,23 @@
       <c r="B17">
         <f>( (V_OUT*V_IN)-V_OUT )/(V_IN*K*f_S)  + R_OND</f>
         <v>66761.617876057877</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <f>K*R_ON_ACT/V_IN</f>
+        <v>1.9909909909909911E-7</v>
       </c>
     </row>
   </sheetData>
@@ -795,21 +821,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,14 +859,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137A78D3-6104-4FD4-B82B-51466FC13F3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57803732-0648-4297-8F65-CB29FE6743D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -848,4 +866,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137A78D3-6104-4FD4-B82B-51466FC13F3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
5V External Buck Done (#7)
</commit_message>
<xml_diff>
--- a/Power_Board_2/Calculations/5V_buck.xlsx
+++ b/Power_Board_2/Calculations/5V_buck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvicca0-my.sharepoint.com/personal/poornack_uvicca0_onmicrosoft_com/Documents/University/Clubs/AUVic/Hardware/PCB-Power_Board_2/Power_Board_2/Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{96FACF96-6EB4-48BA-A4BA-9FAB68A7D684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06C6A0B3-DA3C-49F1-9C0B-AF32DDE05920}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{96FACF96-6EB4-48BA-A4BA-9FAB68A7D684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7CF08298-9F28-453C-91B0-3518F2637AE9}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="16440" xr2:uid="{C6339F42-7D1E-4B11-8B04-09094EF93EB8}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="f_S">Sheet1!$B$7</definedName>
     <definedName name="K">Sheet1!$B$6</definedName>
     <definedName name="R_ON">Sheet1!$B$17</definedName>
+    <definedName name="R_ON_ACT">Sheet1!$B$18</definedName>
     <definedName name="R_OND">Sheet1!$B$16</definedName>
     <definedName name="V_IN">Sheet1!$B$5</definedName>
     <definedName name="V_INMAX">Sheet1!$B$4</definedName>
@@ -35,7 +36,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Calculating R_ON</t>
   </si>
@@ -79,6 +82,12 @@
   </si>
   <si>
     <t>f_SMAX</t>
+  </si>
+  <si>
+    <t>R_ON_ACT</t>
+  </si>
+  <si>
+    <t>t_ON</t>
   </si>
 </sst>
 </file>
@@ -116,10 +125,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10EE0DC-C48A-41CB-95F2-10E1DAB19583}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,11 +455,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -488,7 +497,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1E-10</v>
       </c>
     </row>
@@ -496,7 +505,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>825000</v>
       </c>
     </row>
@@ -543,6 +552,23 @@
       <c r="B17">
         <f>( (V_OUT*V_IN)-V_OUT )/(V_IN*K*f_S)  + R_OND</f>
         <v>66761.617876057877</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <f>K*R_ON_ACT/V_IN</f>
+        <v>1.9909909909909911E-7</v>
       </c>
     </row>
   </sheetData>
@@ -795,21 +821,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,14 +859,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137A78D3-6104-4FD4-B82B-51466FC13F3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57803732-0648-4297-8F65-CB29FE6743D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -848,4 +866,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137A78D3-6104-4FD4-B82B-51466FC13F3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>